<commit_message>
Get daily reddit data: Tue Dec 19 08:08:25 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_24.xlsx
+++ b/data/2023_12_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C460"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2709 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>18lwcli</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Does this count as a Christmas set??</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lwcli</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>18lvscu</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Very proud of the progress I've made this year - gel overlay / polygel</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lvscu</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>18lvot0</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Winter nails! I’m so in love with these press ons!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7jj6us8d877c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>18lvasz</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Fake nails 🌹🖤</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wp0vx40477c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>18lumv2</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Why can I peel my Gel and Dip polish off but not acrylic?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lumv2/why_can_i_peel_my_gel_and_dip_polish_off_but_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>18lu8bq</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Christmas, New Years mash up</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lu8bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18lu4sz</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Christmas set…</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lu4sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>18ltn59</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>merry xmas :)</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zum1wsl8n67c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18ltlbg</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Opinions? I've got mixed feelings</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ltlbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18ltbul</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>incredibly happy with this set!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ltbul</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>18lt3ys</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rx9zrf33i67c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>18lt2a7</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>This set needs to last through Christmas, anniversary, and New Years, so I had to get something flexible 🎄</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lt2a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18lsyxm</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Holiday nails ❄️</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yax08c3tg67c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18lswa5</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Most expensive ($115) but gorgeous holiday set I’ve ever gotten!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lswa5</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18lsh2g</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Silver nails</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blmngflcc67c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18lsli1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Pics don't do it justice but La Colors "Pink Sugar" is my all time favorite "nude"</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lsli1</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18lri3e</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Need inspo</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwn3rkuh367c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18lr5f1</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>noticed this little bump on my nail after being too harsh with the nail drill, can I continue to do work on them or should i let it fully heal/grow out?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lr5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18lpft9</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Gel manicure at home?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lpft9/gel_manicure_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18ls63y</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Nails for the holidays?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xb2hd6ig967c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18lrydd</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Really happy with my Christmas nails! Rubber gel base and colored shellac done by me 💅</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pjdtx5k767c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18lru72</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>2nd Set of Holiday Nails ☃️❄️🎄</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lru72</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18lr7ws</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dainty Gold Snowflakes </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/idy4hl31167c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18lr5ik</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Love my cat eye nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/secq2yee067c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18lr35s</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Aspiring nail tech. Do I have potential?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lr35s</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18lqzck</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhh5v9xty57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18lqyyp</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>First manicure in 2 years!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lqyyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18lqsqg</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Snowflakes &amp; sweaters 🎄</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzkhk1ebx57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18lq79d</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Christmas nails with insistent cat tax</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2npe1je5s57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18lpl1m</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Subtle Frosty Nails</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofy9n0hvm57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18lpac4</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>some recent nails sets I’ve done ✨ I specialize in structured gel overlays and these are all on natural nails</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lpac4</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18lpa1v</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lpa1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>18loxnb</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>The holiday nail on my dominant hand vs non-dominant hand 🤣</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18loxnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>18louvo</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Favorite brands?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18louvo/favorite_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18lotzz</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Elegant Ballet Nails or Cool Girl Vibes? Or both?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3u076fzig57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>18loawi</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>My 1st swoop French</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ciyao601c57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>18lo81x</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Silk Wraps Fraying</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mans2cvcb57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18lnxrb</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Christmas nails ♥️</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p18aifz857c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>18lnnie</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Cozy but fancy 🤌🏼🤌🏼🤌🏼 by @tank__nails on IG</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lnnie</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>18lnibe</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>new set!! i’m so in love with them omg</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lnibe</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>18ln8b1</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Stamping : Stamping gel or stamping polish?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ln8b1/stamping_stamping_gel_or_stamping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>18lmyh3</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Can I put peel off basecoat and regular polish (holotaco) over my tips with dip?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lmyh3/can_i_put_peel_off_basecoat_and_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>18lmpra</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I have to cut off monthly trips to the nail salon for fills from my budget. What is the best press-on nails?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lmpra/i_have_to_cut_off_monthly_trips_to_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>18lmhtr</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>I love this new gel polish. I was going to add a gold French tip but ran out of time.</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lmhtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>18lmgq5</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>2nd ever manicure! Not going into the office for the next two weeks so figured I could go more bold :)</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6myan3vbx47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>18lmg7j</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>christmas set!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6w8petcx47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>18lmeqv</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Since we’re all sharing, here are my Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep3diwh2x47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>18lmddx</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Christmas nails for my third set of gel x</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lmddx</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>18lm9iq</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Honorary Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lm9iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>18lm8c2</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Are these good adhesives for press on nails?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gybcbksv47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18lm482</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>I did this set for my girlfriend - how cute is the lil gnome!!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea63b2jwu47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>18llvu8</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Can I use nail polish over hard gel?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18llvu8/can_i_use_nail_polish_over_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18llokn</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Holiday Nails ✨</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4bxa5klr47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18lllga</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Balerina 🩰❄️ Handpainted 🖌️</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cex2ihnxq47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18llf3d</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Tiny Bats in Santa Hats!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18llf3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>18ll17u</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Someone asked what the other hand on my frenchies looks like.</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55kkly7om47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>18lkyum</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>My first ever Christmas set! I’m in love 🌲❄️</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lkyum</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18lkp0h</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Holly Jolly</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xirn4ig6k47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18ljdfk</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>did these myself</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4meu8wsfa47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>18licq4</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Begginer wants to start doing nails</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18licq4/begginer_wants_to_start_doing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>18lk85s</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Short Gel X</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lk85s</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>18ljppz</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>ghibli nails this month 💛</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ljppz</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>18ljhmi</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>my nail tech popped off today 😍🎄$75 including tip, new jersey</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3awfne29b47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>18lis7j</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>My final Christmas set of the season!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lis7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18linwh</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Press on Help</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18linwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>18li9ps</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>First time getting gel so satisfied</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18li9ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>18lhsyr</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Second set ever, I'm obsessed!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lhsyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18lhlgj</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Christmas French!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y92uehcx37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>18lh1ev</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>first time doing acrylics on myself. howd i do?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lh1ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18le07t</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I’m new to making press on sets / nail art in general.</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgewpfa7737c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>18lgezz</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>A little Monday humor... when you realize your nails match the beef jerky...🙃</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sipj7epuo37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>18lga0n</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Orange chrome nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lga0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>18lfwt9</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Finally found Christmas nails I like (did them myself)</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lfwt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>18lfi1b</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Please ignore my dinner in the background. Its a new nails day!!!!🎉🎉🥳🥳</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hphwds75i37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>18lf05f</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>The manicure I specially did for Christmas, wishing everyone a Merry Christmas.</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lf05f</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>18ldxbl</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>It took me hours to do, but I’m obsessed.</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ldxbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>18ldlj4</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>This was my first time getting my nails done for no reason, I feel so fancy</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ldlj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18lcgvm</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>PLEASE ANSWER ASAP what do I tell my nail tech?!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lcgvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>18lcgdc</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>how to remove press-on nails???</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lcgdc/how_to_remove_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>18ldccr</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>My first ever Frenchies on myself, I think I did really good ! What do you think ?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb3w5b3b237c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18ldbuh</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>How to fix dry/cracked cuticles?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ldbuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>18lbzfu</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>How can I care for my nails with vitamin issues.</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lbzfu/how_can_i_care_for_my_nails_with_vitamin_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>18l75uu</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Can someone help me figure out this nail color?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b85a8nrn17c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18lcmx7</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>French for the holidays!!</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2tsky6zw27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>18lcgrk</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Green and Gold ✨️</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lcgrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>18lcch8</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Gel x(mas) beginner!</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lcch8</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>18lc39v</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Cute 😍</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b7xyzyys27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>18lbw0w</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>self taught 19 y/o “tech”</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lbw0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>18lb82q</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc51trldm27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>18labvm</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>question about my nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18labvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>18l9xlv</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Wintry Mix</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18l9xlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>18l9snk</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>I have the best nail tech</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwahfm4bb27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>18l9do7</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18l9do7</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>18l92ce</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Recommendations for UV gloves?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18l92ce/recommendations_for_uv_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>18l90do</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Recommendations for E-Files to remove gel polish?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18l90do/recommendations_for_efiles_to_remove_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>18l8ye2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Question 🙋🏻‍♀️ I do my own fake nails for special occasions because I can’t function day today wearing them but I do like if they last maybe a couple of days and most certainly for the event.</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18l8ye2/question_i_do_my_own_fake_nails_for_special/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>18l8ssu</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Couldn’t decide which Christmas style to do, so I did a bunch!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqy3uqj4327c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>18l8l4t</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>🖤✨</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znpy7b4a127c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>18l8cls</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Jolly Fat Man</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18l8cls</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>18l8644</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Christmas cookies nails 🍫🍭</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18l8644</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>18lvtd3</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>a quick palate cleanser before xmas 🤍</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff4q78nv977c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>18lvozb</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>ILNP Pixie Party has got me into iridescent nail polish!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lvozb</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>18lukpw</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Revlon smell good series...</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upc2n3gdw67c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>18lrrmo</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Little bit of a palate cleanser - does this count as strawberry milk? 🍓</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lrrmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>18lr3sy</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Rainy Day Retro Teal</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uv1abkrz57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>18lnjym</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Chrome polish suggestions?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18lnjym/chrome_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>18lnf7y</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>ILNP Black Friday skittle!</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4h16q9u457c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>18lmlz0</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Snake eyes</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lmlz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>18ll9tc</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>First time my glitter polish hasn’t looked like utter trash 😅</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95403lfio47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>18ll72w</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Every color I bought from Cirque in the past year is on clearance now 😭💸</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19apt6vxn47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18ll2ob</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Something a bit regal</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ll2ob/something_a_bit_regal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18ll0tv</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Some Winter berry shades</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ll0tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18lkt8d</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Rose gold nails</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c22p20v0l47c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>18lkn4h</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Flakie Brown</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lkn4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18lkicw</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Feeling festive (and hoping for some polish under the tree)</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wojckx7ti47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18ljokg</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Artemis Deathkiss</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2v5l48vnc47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18lhw84</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Been sleepin on Majolica!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6gvm7bkz37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18lguyu</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>First holiday set with a red skittle.</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/JOIb2YP</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>18lgm7w</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Neon Christmas vibes</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sh2o2uw8q37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18lg15s</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Light it Up - like having mini candle nails lol 🕯️🔥</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6j4xa9pwl37c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18lfzzh</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Just showing off 🫶🏼 they’ve been needing a trim every week</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lfzzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18lfvha</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Polish goopier in the winter(cold weather)?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0pvtqzrk37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>18lfml6</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>So excited to finally try the famous ILNP Rosewater</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lfml6</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>18lfjwh</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>first magnetic velvet attempt</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lfjwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18lejr8</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Serpentine (cirque colors)- favorite I’ve tried</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8l0x8s6b37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18le6p9</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Turning stones into opals: chrome powder on cremes</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18le6p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18ldl37</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Festive nails</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ldl37</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18ld7oc</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Ranking all of the brands I tried in 2023: The “Every Rose Has Its Thorn” Chapter - Part 1</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ld7oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18ld05i</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>[Question] Does polish thinner work on quick dry topcoats? What is the best way to extend the life of a quick dry topcoat?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ld05i/question_does_polish_thinner_work_on_quick_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18lcz2f</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Can anybody colour match this?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lcz2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18lcu82</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Weekly check-in thread for those on a no buy, low buy, etc.</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18lcu82/weekly_checkin_thread_for_those_on_a_no_buy_low/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>18lccva</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Trying to get into the festive spirit, loving this metallic green!</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czhmfgovu27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18lbx35</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Jumping on the Holiday Bandwagon</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3n86bpqnr27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18lbt2p</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>{PR} The Best in Snow Collection by KB Shimmer</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g92jhextq27c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>18lbdyv</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Need a dupe!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lbdyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18lba4n</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>OPI - Pixel Dust</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lba4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18lb50m</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>The Sparkle Has Arrived</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ymOJMmV</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18la08q</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Wintry Mix</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18la08q</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18l9o8p</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Holo Heaven!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rdlctlx8a27c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18l91y0</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Recommendations for UV gloves?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18l91y0/recommendations_for_uv_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18l909i</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Glampire!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18l909i</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>18l8l6z</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Recommendations for E-Files to remove gel polish?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18l8l6z/recommendations_for_efiles_to_remove_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>18l8e03</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I’ve come a long way!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18l8e03</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>18l79ha</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Snowing here today!</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vo6ncjyro17c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>18l63bi</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18l63bi/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>18lvbir</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Merry Christmas! 🖤✨</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ule8wt68477c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>18lsqnl</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Soft glitter pink acrylic and snowflakes.</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0cg7w9qe67c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>18ls0gz</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Went a little crazy this year for Christmas</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn9pv6x3867c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18lpwij</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Kuromi Inspired Kids Gel Manicure</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2xq2a6jp57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>18lp98k</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Christmas 🎄 Nails</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4j3mmo92k57c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>18lnmoh</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Cozy but fancy 🤌🏼🤌🏼🤌🏼 by @tank__nails on IG</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lnmoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>18lkb97</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Inspired by sydney3threenails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7qcq27ch47c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>18liesf</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>A little rushed but still cute Imo. Christmas has been very busy for me this year.</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr5oqey8347c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>18lheht</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19c9mkgwv37c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>18lff82</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>A little Christmas sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lff82</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>18ldz8c</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svzr60qz637c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>18ldaeb</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Christmas theme last year was a nice blue 💙 ( ChiChi Nails in Canada ) Merry Christmas Everyone 🎅 🎄</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py8rjaew137c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>18l52bn</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>ChiChiNails in Canada ♡ i love my nail tech 🤍😭 a bugz lyfe 🐛</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30d643ykz07c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>18l51s4</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>soooo I love with the sets my nail tech gives me ♡ ChiChiNails in Canada - 🤍🦕</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bphzzngez07c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec 20 08:06:52 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_24.xlsx
+++ b/data/2023_12_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C460"/>
+  <dimension ref="A1:C604"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8253,6 +8253,2454 @@
         </is>
       </c>
     </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>18moppd</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18moppd</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>18mo0ch</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Holiday chrome ❄️</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dzjxxjk59e7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>18mnac4</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Getting a manicure after acrylics are removed</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18mnac4/getting_a_manicure_after_acrylics_are_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>18mn7s2</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Gel to acrylic?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18mn7s2/gel_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>18mm58a</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Broke some nails so I had to go get my nails done, really liking the color she picked out for me 🩷</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mm58a</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>18mkte8</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>How do you güys feel about press ons? 💅🏿</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/145c8zfrdd7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>18mjhsm</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>can anyone recommend a more natural base color?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6fftw2x1d7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>18mhu73</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Should I push my cuticles back? Or should I be trimming them?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mhu73</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>18mfpff</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>My mum wanted to show her nails! She was inspired by my red chrome set!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x7q6vhf5c7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>18mechr</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Angry technician/owner</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mechr</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>18mb3q2</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Fixing scuffed gel</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mb3q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>18m9fh4</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Dizzy with monomer</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m9fh4/dizzy_with_monomer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>18m7tre</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Red-y for the Holidays!</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iecag03jha7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>18m7fyk</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>My nails are in the roughest shape of my life! I need some sort of protection while they grow but also want them to look cute for now. I've never had anything done at a nail salon, what should I ask for?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m7fyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>18m6nbb</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Nail salon said gel x extension removal would be $75</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m6nbb/nail_salon_said_gel_x_extension_removal_would_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>18ml7xr</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>First time using proper fake nails. Should the tips be pressed down more?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ml7xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>18mku6r</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>My Xmas/ Doja Cat concert nails</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h53rhwtydd7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>18mkgcx</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Christmas/birthday set</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mkgcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>18mk48q</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Burgundy for Winter</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwypavpj7d7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>18miz6d</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Dip nails only last a week</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18miz6d/dip_nails_only_last_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>18mix1m</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>New set I made</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mix1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>18mij8e</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>December chrome</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mij8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>18mie2d</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>first post, favorite recent sets</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mie2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>18mh2jv</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>why is airbrushing so hard!!!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18mh2jv/why_is_airbrushing_so_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>18mgsnf</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Quick rant about nailtek</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18mgsnf/quick_rant_about_nailtek/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>18mg5vx</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>first time trying press ons! ($35)</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nbkypy39c7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>18mg2y4</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Red Chrome French</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zobq4jte8c7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>18mfnos</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Will a regular gel base coat stick on clear fake nails under UV light?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18mfnos/will_a_regular_gel_base_coat_stick_on_clear_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>18mfn0v</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Christmas ready!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t0vmkmw4c7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>18mfgmp</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>New here🫶 some of my fav sets I’ve done for me/my friends 🥰</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mfgmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>18marvt</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Which products/techniques/tools can I use to recreate similar designs to these on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18marvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>18mcj44</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>lil minimal candy cane manicure I did on myself 🎄</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mcj44</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>18mehml</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Happy Holidays to all❤️</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo2v52hwvb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>18me8du</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>What is your go to color for your skin tone?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18me8du/what_is_your_go_to_color_for_your_skin_tone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>18mdvxe</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Latest and greatest, I reckon. You can kinda see my natural nail underneath but it's not too obvs.</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mdvxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>18mdsvz</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i7a924fqb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>18mdrxu</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>My take on festive. Hard gel on natural plate.</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mdrxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>18mdfmm</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Simple ones for the greatest lady</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phtmdn9knb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>18mdbtb</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Help meeee</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fpce86smb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>18md5bt</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>‘prawn cocktail’ anyone? 🦐🍸 handpainted by me</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1gy90kelb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>18md31a</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Let it glow set</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18md31a</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>18mcrlq</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Advice on Press Ons</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czgyqvdjib7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>18mcpjy</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in a long time!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mcpjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>18mcn5t</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I realize I should’ve did the glitter last after the fact. 😂</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyx21abkhb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>18mckzp</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>French Cat Eye</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mckzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>18mcevq</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Winter nail art</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mcevq</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>18mcbul</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jb4cwvafb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>18mcajv</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Obsessed with this holo gel!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/osowdgu0fb7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>18mc3v1</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>O Christmas Tree</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ij28p9mdb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>18mbtk3</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Regular magnetic iridescent nail polish</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/C025Qg0Lf0d/?igshid=MzRlODBiNWFlZA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>18mbsl4</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Festive nails, light bulbs glow in the dark 🙃</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax4m5le9bb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>18mam1u</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>First time doing an ombré for my nails! Definitely ended up being more of a flat color though</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnu5yg0d2b7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>18maca3</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My nail tech is amazing! Each one of this flowers is painted by hand! I'm amazed by her talent</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18maca3</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>18ma5xb</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Second time doing acrylics on myself</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ma5xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>18m9sx3</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Cute Snowflakes</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpe2eekcwa7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>18m9oqb</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>How do yall do straight lines i’m losing my mind LMAO</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl8oqpygva7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>18m9dhk</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>These came out so cute!!</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m9dhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>18m9a7q</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>How to make press ons less transparent</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jty63awhsa7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>18m8goh</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>most chaotic set i’ve done, but i love how festive it is</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m8goh</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>18m85ig</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>first morning coffee in my new renovated kitchen &amp; home! 💁🏾‍♀️☕️🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc69gne1ka7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>18m6ztx</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>my first nail stamp attempt!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m6ztx</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>18m6kbl</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Nail art hiiiiiii</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys24lna18a7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>18m6brb</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Fake nail question</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m6brb/fake_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>18m6aos</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>✨❄️✨</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwcb7j206a7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>18m60ar</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Manicure day ❤️💅</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dakc3ses3a7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>18m5x9x</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>My Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m5x9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>18m5lv1</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Drill with vacuum system (Medicool Pro Vac) for manicure and Sunflower question</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m5lv1/drill_with_vacuum_system_medicool_pro_vac_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>18m5l5b</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Christmas Nails to change up my routine</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k0k9hlj0a7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>18m1d7o</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Clueless BF needs advice on buying a gift for girlfriend</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m1d7o/clueless_bf_needs_advice_on_buying_a_gift_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>18m56h6</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Merry Christmas all! 🎅🏼🎄</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k398y6tix97c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>18m4uhv</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Pink/Mauve Color Block 💕</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m4uhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>18m4mpc</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>‘Tis the season…</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m4mpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>18m4mp4</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Terrible salons lately</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m4mp4/terrible_salons_lately/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>18m4kfg</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Builder gel lifting instantly</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc55o10us97c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>18m3eil</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Dehydrator + primer + peel off base?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m3eil/dehydrator_primer_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>18m38sy</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>❄️ My Christmas Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m38sy</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>18m2h9m</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m2h9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>18m2bk4</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Christmas feelings on todays client.</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e51pvm8ua97c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>18m1z7r</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>i’ve been doing dip powder and would luv to hear your thoughts,</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m1z7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>18m1ygg</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>My Nails Without Polish 12/19/23</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z8w22dh797c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>18m1na3</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Loving this Mango colour while on holiday</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fj7nr4u497c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>18luxh8</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Allergic to gel, so Old School lacquer on natural nails</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f08age40077c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>18m16qp</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>I have developed a sensitivity to gel nail glue. Can I use regular glue with Apres Gel-X?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18m16qp/i_have_developed_a_sensitivity_to_gel_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>18lzvig</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Loving my holiday nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y06dvaban87c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>18lz7kn</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>I got to my BF’s nails 👀</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65b09iisf87c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>18lz7k9</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Green and glittery for Christmas</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrf4k7ksf87c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>18lx5pa</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Salon done frenchies &lt;3</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lx5pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>18lwv19</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Finished self done set ! &lt;3</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lwv19</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>18lwsvq</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Favorite cuticle oil &amp; softener?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18lwsvq/favorite_cuticle_oil_softener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>18mo5ss</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Anyone Else used Nail Aid polish and had a Severe allergic reaction similar to HEMA Acylate reaction with gel polishes?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mo5ss/anyone_else_used_nail_aid_polish_and_had_a_severe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>18mntyo</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Nails after gel removal</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mntyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>18mngnr</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Magic Forest by Tuesday in Love</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ik7olyh3e7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>18mm4ja</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Soaking nails in jojoba?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mm4ja/soaking_nails_in_jojoba/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>18mlf40</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Christmas Mani 🎄</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mlf40</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>18mkh1b</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Mooncat polishes that are worth it?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mkh1b/mooncat_polishes_that_are_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>18mj7z1</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>OPI Skate to the party</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl6em68izc7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>18mj6zi</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Which type of nail for short term wear?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mj6zi/which_type_of_nail_for_short_term_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>18mijk4</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>My Second Mooncat Order!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sgpgfoltc7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>18mhn0y</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Can't Believe the Shifts</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mhn0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>18mhmf0</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>ISO green polishes with blue shimmer</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mhmf0/iso_green_polishes_with_blue_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>18mhjc2</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Purple manicure, but make it festive 💜🎁</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mhjc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>18mgalu</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>A Dragon Without a Rider is a Tragedy</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mgalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>18mfosm</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Horror story that just happened with a non- nail nerd friend</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mfosm/horror_story_that_just_happened_with_a_non_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>18mf1q2</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>A maroon and forest set</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2rmk16xzb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>18meris</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>RIP 😭</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udves2x0yb7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>18me0jy</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Wintery fun in the snow</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18me0jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>18mdih8</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Best ridge fillers ?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mdih8/best_ridge_fillers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>18mas0a</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>First time seeing this sub…</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mas0a/first_time_seeing_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>18ma329</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>La Colors Princess Vibes 😍</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ogp0qpcfya7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>18md6ud</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Dimension Nails Vanilla Almond Milk - nice, neutral, milky white</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18md6ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>18mcoiw</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>BKL Buzzmas Spoiler: Lucien</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mcoiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>18mclfq</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>lil minimal candy cane manicure I did on myself 🎄</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mclfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>18mck5f</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Ranking all the brands I tried in 2023: The “Every Rose Has Its Thorn” Chapter - Part 2!!!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mck5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>18mcjsc</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Prawn ‘cocktail’ anyone? (handpainted by me)</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mcjsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>18mbv31</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Roast my skittle</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mbv31</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>18mbpot</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Before I go full Christmas nails, I just wanted to say this is week 3(!) of this manicure.</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1g4pm4nab7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>18maa6x</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>First attempt with magnetic polish</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnx1b4mvza7c1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>18m8twg</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Pastel Wintry Vibes</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m8twg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>18m8hmq</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>My tree cookie earrings almost perfectly match this topper!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbpksdllma7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>18m7zst</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Macchiato Cloud</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9lsmwwoia7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>18m7kzs</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>First self gel mani</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m7kzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>18m76wk</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>What brush do u prefer?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18m76wk/what_brush_do_u_prefer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>18m6uzn</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Someone convince me I don’t need two similar Cirques 🌵💚</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqq93fr7aa7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>18m6epv</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>It looks like a different polish in every picture</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m6epv</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>18m614h</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Red, gold, and green for Christmas</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m614h</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>18m5npq</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Moody palate cleanser before Christmas nails 🖤</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtop8g731a7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>18m50tx</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>one last mini mani dump + reviews for the year</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m50tx</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>18m4tzq</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Something a bit regal</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18m4tzq/something_a_bit_regal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>18m4rf6</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Does Orly Nail Rescue Expire?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnycwm1au97c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>18m4iwc</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Gel polish application method alternatives?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18m4iwc/gel_polish_application_method_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>18m2x90</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Matcha latte looking beautiful</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as68y7cvf97c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>18m1hh1</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I miss them 😔</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojal8rcd397c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>18m0d74</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>My wife’s Christmas French Tips, including some Holly!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhlz1efjs87c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>18lxd09</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>(First pic is a salon mani) Never painted my own nails before. “Upgraded” a mani for Christmas.</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lxd09</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>18mo0v7</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Red @alicasmd</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rpbs2xra9e7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>18mkogk</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Fluorescent fire 🔥😍😍 nails made by me for a client 🥰</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgejqouicd7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>18mke7a</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>My chrimis nails</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mke7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>18md5dz</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Let it glow</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18md5dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>18mckhv</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>lil minimal candy cane manicure I did on myself 🎄</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mckhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>18m56tg</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Merry Christmas all! 🎅🏼🎄</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jgo6t8lx97c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>18m466a</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Mani by Me: 3D Sculpted Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m466a</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>18m2r1l</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>These fulfilled this year's Christmas Wish!!</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18m2r1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>18lyjfc</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>From the inspo to the nails set</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18lyjfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>18lxhi9</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>love my christmas nails✨</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m9hu05iiu77c1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec 21 08:08:13 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_24.xlsx
+++ b/data/2023_12_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C604"/>
+  <dimension ref="A1:C758"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10701,6 +10701,2624 @@
         </is>
       </c>
     </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>18ngl57</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP! I am STRUGGLING with cat eye gels? Is my magnet not strong enough? </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r0kn89smfl7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>18nfxkr</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Red matte Christmas 🎄 nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fpxjp5v8l7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>18nfwy8</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>I don’t know much about nails, are these well done? they’re almost a week old.</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nfwy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>18nfv2q</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Are these as bad as I think they are?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nfv2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>18nff91</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Happy Holidays!! 💖</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nff91</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>18nf55e</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>looking for the perfect red but always playin safe 🥹</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k78c8k3n0l7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>18nf46e</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Should dip nails chip?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgg8zplh0l7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>18nea0s</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>first time trying gel x</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/117o0bixrk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>18ne7bp</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Simple frenchie by me❤️</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ne7bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>18ne6b3</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>newest press on set 🎀🖤</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ne6b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>18ndqu6</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Press on brands recommendations</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ndqu6/press_on_brands_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>18nd9mq</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Too early for New Years nails?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nd9mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>18nclzu</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Glamnetic press-ons in the style “Juicy”</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k6ayu828ck7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>18nbjoc</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>My nails often split like this</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gt75f5b2k7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>18nbffm</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Festive nails! 🎄</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu3m04e81k7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>18nb8hk</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>My DIY Holiday Nails. Still practicing my line work. 😅🩷</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbyrgcufzj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>18nb16i</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>My nails to xmas</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqee41njxj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>18navxi</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18navxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>18naudj</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Winter nails for my mom (⁠人⁠ ⁠•͈⁠ᴗ⁠•͈⁠)</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18naudj</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>18namhu</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Christmas Red</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqbtfoqttj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>18naixs</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Intrusive thoughts</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18naixs/intrusive_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>18na94d</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>How to make press ons last</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18na94d/how_to_make_press_ons_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>18n9wt5</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Grinch vibes</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwqiwwdenj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>18n9ued</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>My husband picks his nail beds and wants to quit</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18n9ued/my_husband_picks_his_nail_beds_and_wants_to_quit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>18n9lsa</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Back with my fresh set</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvzatewokj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>18n9isy</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Christmas press ons 🥰</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n9isy</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>18n8qtb</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>ready for Christmas!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q6vrpnedj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>18n8kyc</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>When Halloween is your jam but, you're still feeling the X-mas spirit</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n8kyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>18n8hbl</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>How were these made?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n8hbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>18n8ej6</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Got my nails done for Christmas</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0tgtljnaj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>18n7h8j</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>First attempt at ✨️glitter✨️ dip nails (Christmas edition)</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n7h8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>18n7fp5</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Sugar Plum Princess Fairy</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hau1tmw2j7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>18n6xzv</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Cat eye butterfly nails.</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqsuln30zi7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>18n6rwe</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>More Christmas</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n6rwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>18n6lhf</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Did some Christmas themed mails!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n6lhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>18n6c1c</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Latest 6 sets 💅</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xkvr0v9ui7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>18n67sq</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>New christmas set</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s3s84fcti7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>18n5yj5</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Mommy and mini matching nails.</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emtuvwwcri7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>18n5k3k</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>More information on caption please help!!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5kpy0m9oi7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>18n5h6i</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Cat eye aurora nails 🦄</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if92bdloni7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>18n4yb4</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Nails I've done recently...</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n4yb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>18n46d9</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Christmas nail art for December</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n46d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>18n42uv</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Festive nails with glitter and a little bow🎀</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n42uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>18n3x5l</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>How bad is it?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b392w7njbi7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>18n329q</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>My Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n329q</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>18n2uvv</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>I thought i was bad at water marbling until i used polishes from the same brand with the same formula</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3ggccyc3i7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>18n2pq1</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Cat eye and chrome</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pkx3xv92i7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>18n2kii</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>I tried to do swrils but they didnt come out as swirly as expected but they still look aesthetic tho</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbqbjkr61i7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>18n2clo</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Soak in water before gel polish application?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18n2clo/soak_in_water_before_gel_polish_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>18n26o5</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Do these look good or</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc373khcyh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>18n1ywu</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k94oqjrwh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>18n1n4g</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Merry and Bright 🎄❄️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6olhmsauh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>18n1ikj</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Christmas nails ❤️✨️</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s00fl3ydth7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>18n1gwb</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>my nail broke last night</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n1gwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>18n1exc</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>second go at gel x with nail art</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n1exc</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>18n1alz</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Gold middle finger just for “fuck you” purposes.</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zy5j2rsrh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>18n15jf</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Classy and simple Christmas nails this year 🥰 I love them</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n15jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>18n14oa</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkazt3cmqh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>18n0wfd</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I did a floral set on a friend this week</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9atqipjzoh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>18n0dou</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>First time getting Apres nails</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n0dou</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>18n05tv</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>A perfect red color</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ib6ursnjh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>18n011q</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Is this a good shape or does it need a taller apex</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04tj7gtpih7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>18mzf8f</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>My updated Christmas nails ❤💚</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mzf8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>18myuqf</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Christmas wrapping paper nails!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q20j55bw9h7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>18mp9by</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>New to nails, what do I ask for at the salon?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18mp9by/new_to_nails_what_do_i_ask_for_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>18mquu9</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Does anyone know how this could happen?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wk82spug7f7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>18myacy</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>First attempt at aquarium nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/87prg57k5h7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>18mx90z</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Matte and shiny ✨</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94dj9b8nxg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>18mx2cd</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>I’m dreaming of a white christmas ❄️✨🤍</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lxpvjc7wg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>18mwgzk</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Can you apply gel polish over cured gel polish?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gj8hhvprg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>18mvoth</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Christmas/New Years Nails</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mvoth</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>18mv7ls</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Fresh set for the holidays, Merry Crystler. 🎁💅❄️</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zecgw76chg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>18mv3pb</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>New lunar year is the year of a green dragon 🐉</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ook8nvzdgg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>18mv06o</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Applied press ons for the first time ever...how fake do they look?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz7bnbnkfg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>18mudv1</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Christmas nails 💅</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8ei0am2ag7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>18mt9ap</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Holiday French Nails</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pphvpuq2zf7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>18msy59</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>A set that I made today / first time making a ribbon from solid pvc gel</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18msy59</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>18mr2gc</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>merry christmas everyone ❤️</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mp22af2af7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>18mq0sf</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Got these snowy claws done today! She freehand painted the awesome snowman!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v964l2cxe7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>18mphkz</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>DIY press on nails 💅</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/18u34bnpqe7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>18nhshv</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>A dupe for this polish?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyetxi7ptl7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>18nfjqd</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>I want to post my review of the year but I’ve done my nails 152 times this year so far. 😭</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nfjqd/i_want_to_post_my_review_of_the_year_but_ive_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>18nf4uu</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Nails Inc London at Dollar Tree!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nf4uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>18nf3ar</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Did I do the velvet thing???</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/na5dn9b80l7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>18ney6n</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I go extra for the holidays</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0ilau4tyk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>18nejb3</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Red and gold holiday mani 💅🏽</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jtbla29ouk7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>18nee2r</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>First time stamping!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nee2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>18ndpun</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Fav gold (or generally warm-toned) holo top coat?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ndpun/fav_gold_or_generally_warmtoned_holo_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>18ndepu</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Christmas tree nails 🎄</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xtw4vrqjk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>18ndcuq</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>dvn dust to dust amethyst🔮🪻</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i99x4o94jk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>18ncfc6</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>A newbie’s year in review!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ncfc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>18nc9rh</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>*cough cough* I’m sick</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fd0idb19k7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>18nbt0g</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>First magnetic mani! Yay Christmas!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k9ztu62p4k7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>18nbjli</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Jewel tones 💎✨</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nbjli</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>18nbb0i</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Anyone ever try Dip?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nbb0i/anyone_ever_try_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>18naqjn</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Graduation Nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18naqjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>18naf6r</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Magnetic troubleshooting?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpnr02tyrj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>18na3el</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Did a frosted opal look</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytxnhr3woj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>18n9ob8</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>PSA: Holo Taco Not Pressed can cause staining even with base coat</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fgz6tkblj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>18n94qk</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Oh Christmas tree!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n94qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>18n8us7</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>I WILL make this magnetic polish stay!!</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n8us7</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>18n8i4v</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Pink Wintery</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n8i4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>18n7fj9</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>How long does Peely Base last on you?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqdu42cv2j7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>18n74ut</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Looking for not quite Mooncat Misery/Smokescreen</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18n74ut/looking_for_not_quite_mooncat_miserysmokescreen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>18n6rfl</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>How quick is quick dry top coat?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18n6rfl/how_quick_is_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>18n6iiy</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Clear Naked Nail Flex :p</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n6iiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>18n65n4</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Improvised a design</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n65n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>18n5wed</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0q74wtuqi7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>18n5nv8</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>My most festive (and earliest to chip) look this year!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n5nv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>18n5mv7</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Lumen Overpour Mysteries</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/navu74zuoi7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>18n5axm</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>me to literally anyone who will listen:</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n5axm</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>18n4kpx</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Discussion: your favorites this year? Here's my year in review :)</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n4kpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>18n3yki</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>All my Christmas nails from this month</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n3yki</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>18n3elg</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Snowy Footprint Nails</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n3elg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>18n32ux</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>The extent of my holiday decorating this year</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n32ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>18n2d6l</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Another shot of this beautiful shade 💗</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cm8nlznzh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>18n1mbe</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Ranking Every Polish Brand I Tried in 2023: The “I’m Smitten!” Chapter - Part 1</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n1mbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>18n1hxx</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Cirque Colors Clearance Sale</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18n1hxx/cirque_colors_clearance_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>18n1e69</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Angels Flight to Starry Nights</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n1e69</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>18n0r91</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>OPI - Yay Or Neigh</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n0r91</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>18n0pdj</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>🌲🌲</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n0pdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>18n02po</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>How do I get my hands on Glass Frog?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18n02po/how_do_i_get_my_hands_on_glass_frog/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>18mzzbv</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Staining?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mzzbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>18mzk87</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Holo! It’s almost Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mzk87</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>18mz1uy</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Took this sub's advice</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dllstl3hbh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>18myh5m</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Flannel is forever</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18myh5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>18mxybq</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Can we declare blue a Christmas colour?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grcdmkq23h7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>18mxpus</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>{Gifted} Love red reflective too much! 🫣</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mxpus</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>18mxge2</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>My first Christmas set! 🎄</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbx70i67zg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>18mxevh</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Christmas mani and test of a new indie brand!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mxevh</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>18mwwbs</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Just a cozy li'l frosted metals Christmas skittle for my shorties 🎄</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qpynjjxug7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>18mwetk</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Icy nails 💙</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xhvd7p6rg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>18mwdoz</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Christmas nails and my first French</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mwdoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>18mw1u9</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Yet another Christmas mani...can't stop, won't stop!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mw1u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>18mvjth</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Can I reapply base coat without removing old layer?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18mvjth/can_i_reapply_base_coat_without_removing_old_layer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>18mrh7o</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Dupe for this PPU</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18mrh7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>18nf1wz</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>ice pop bears ฅ՞•ﻌ•՞ฅ 𓂃⊹ ִֶָ</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nf1wz</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>18nepqj</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Just finished 😊</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5pn3l5hwk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>18nenec</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>I want to open my handmade press on business early next year but am unsure what price to make it at. what would be a good price for this set? any advice would be appreciated!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vl1dh5olvk7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>18ncd7p</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Doubt anyone here will understand their theme but I love what I did and need to show them off! 😅</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5oua5p4y9k7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>18ncb2a</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Been seeing my nail tech for 8 years and this is my favorite set so far!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld926gvc9k7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>18n7f9w</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Thanks to Lee at Nails of America-heights! He did a great job.</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n7f9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>18n7329</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Happy Holidays</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azl9da140j7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>18n61k6</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Merry Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0a5dkozri7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>18n5nvm</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Snowman Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0a590l2pi7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>18n44rr</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>I made this set to match a clients color analysis 🌈</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmfrldz5di7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>18n1066</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Studio Ghilbi - Spirited Away Nails</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n1066</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>18n0v0y</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Tortoiseshell Nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n0v0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>18n0rxe</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Snow Capped Mountain 🏔️ Peaks w/ Clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n0rxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>18n0pe8</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Full coverage tips, hand painted red holiday edition nails 💅</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkq6el8nnh7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>18n0fnw</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Recent sets I’ve made</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18n0fnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>18myu1i</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas wrapping paper nails! </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0quztdnq9h7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>18mvslw</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Puppy portrait</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ir0u1jr4mg7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>18msn41</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>First attempt at aquarium nails</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/saiq2t3gsf7c1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec 22 08:07:59 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_24.xlsx
+++ b/data/2023_12_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C758"/>
+  <dimension ref="A1:C949"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13319,6 +13319,3253 @@
         </is>
       </c>
     </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>18o9qe1</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Did my nails at the salon after a long time for the holidays!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ad6g1vgys7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>18o8knp</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Simple Christmas nails</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtxya8s8ks7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>18o8ghm</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>To prove that I could</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o8ghm</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>18o89jj</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Christmas skittle</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5jml8wpgs7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>18o81v8</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o81v8</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>18o7y0t</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Did the lady at the salon trick me</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18o7y0t/did_the_lady_at_the_salon_trick_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>18o7kw1</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>❄️🥰</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/22ircgp59s7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>18o7hms</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Found better lighting</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o7hms</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>18o6gxk</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I have NOT learnt my lesson about leaving my gel pot on my desk at mid morning when the sun comes in. This... even with the lid closed 🤪. Is there a flair for "idiot" ??</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6anfre4nxr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>18o6cm3</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Polygel Snoopy set :)</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o6cm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>18o65h3</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I was aiming for Christmas sweater vibes but got bus seats instead. Still not mad.</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucfl4yeeur7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>18o634d</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>blue aura nails 🦋</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/074a52qrtr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>18o5tjq</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Help finding a dip or gel color</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyuhyxg6rr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>18o5ep6</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Manicure chipped within a week?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18o5ep6/manicure_chipped_within_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>18o5ae3</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o5ae3</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>18o56dr</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>What do you think</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a08txn3rkr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>18o54kp</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5evufx9kr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>18o4xdt</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>I love my new set of nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jn6h7f9dir7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>18o4u1a</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Christmas snowflakes ❄️</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o4u1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>18o4tcb</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Love my nail tech 💚</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o4tcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>18o4spn</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Opinions on half moon nails?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18o4spn/opinions_on_half_moon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>18o4dvg</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>✨ Christmas sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev2hgnhbdr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>18o40jl</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Matching set</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2lb2lwx9r7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>18o3rg6</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>It’s almost Christmas! 🎄</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1tsvt1n7r7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>18o3nz1</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>just got these gel-x done 2 days ago and they are already falling off :/</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skri9tfs6r7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>18o3j89</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Help matching a color?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o3j89</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>18o2qco</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>My Christmas nails (Not done by myself)</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o2qco</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>18o2k3r</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Beetles UV lamp</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyl75aoowq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>18o2c2h</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Pearly glitter nails for the winter! Took me so long but I love them</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o2c2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>18o2b7s</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8080mydmuq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>18o28lm</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Salon Won't Give Me a New Set</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o28lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>18o27n1</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>does using multiple layers of gel base coat do anything?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18o27n1/does_using_multiple_layers_of_gel_base_coat_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>18o22mf</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Winter-ish nails ❄️</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o22mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>18o1zhl</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>HELP! Engagement photos + regrowth</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18o1zhl/help_engagement_photos_regrowth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>18o1s12</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Christmas\new year’s set!</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qn3jtr3qq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>18o1klk</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb1p54cdoq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>18o1k1b</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Brown Xmas and new year nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o1k1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>18o1hrk</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Just want to show off my amazing nail tech</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o1hrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>18o1fkm</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Can I have acrylics done on molds of my hands to save time?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18o1fkm/can_i_have_acrylics_done_on_molds_of_my_hands_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>18o0ufd</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>I’m getting my nails done early January, what color/design?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o0ufd</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>18o0j86</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Recs: Nail shape and type of manicure</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvx9yc6xfq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>18o0hgc</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Obsessed with these little deer nails I did today! All hand painted</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqi8jmgifq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>18o0ac1</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>60s Psychedelic Flowers</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crimbiewdq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>18o057r</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Nail Advice</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o057r</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>18nyn2r</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Grown out builder gel. Tips on filing them down with a regular nail file. Then can I fill them in with more gel?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nyn2r/grown_out_builder_gel_tips_on_filing_them_down/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>18nyi52</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Fav DIY of 2023</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nyi52</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>18nyhqz</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>So in love 😻</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcl2s9upzp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>18nygz6</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nygz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>18nyart</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Back to pink!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nyart</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>18nxxzq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>WINTER SET❄️❄️❄️</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9qsqrrcvp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>18nxn53</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nail sticker placement question</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nxn53/nail_sticker_placement_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>18nxghv</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Looking to do nails at home</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nxghv/looking_to_do_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>18nxejy</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Christmas nails for Disney World 🎄🖤🤍</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ole1ld6rp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>18nx9uu</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>I got christmas nails today</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uklw9n4qp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>18nwuw2</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Feeling festive🎄</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5c0wwhzmp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>18nw68d</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>My set for the holidays!!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nw68d</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>18nrd7s</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Allergic to gel and dip</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nrd7s/allergic_to_gel_and_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>18n42au</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>What Treatments are Safe for Acrylates Allergy, and Best Press-on Tabs?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18n42au/what_treatments_are_safe_for_acrylates_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>18nvx3l</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Brown in corner of nails</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nvx3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>18n76wx</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Candy Cane nails!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18n76wx/candy_cane_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>18nauef</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>I have a clubbed thumb. Anyway to get this fixed?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpjvew7tvj7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>18nbb18</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>What do I do about oily and flimsy nails?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nbb18/what_do_i_do_about_oily_and_flimsy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>18nf1to</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Inspired nail arts</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hqxdwstzk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>18nvsi9</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Red velvet nails for a friend</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26ookegmep7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>18nt9ed</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>What service do I need?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nt9ed/what_service_do_i_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>18ntscu</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>winter, gal-inspired nails by me!❄️🤍</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ntscu</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>18nv9dt</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Vacation nails!!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nv9dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>18nv8pn</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Fresh Christmas set 🎄</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5wlxstdap7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>18nv7my</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>A Little Midnight Gobble</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nv7my</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>18nv5om</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>my hands since i started using this cuticle rehab!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nv5om</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>18nup6v</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xeb7ui496p7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>18nufug</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3yrirxa4p7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>18nu4d7</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Beyond obsessed with my chrome nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nu4d7</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>18ntqh8</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>White nails 🤍</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jw62zz9wyo7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>18ntddv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Reattempted snowflakes, slowly getting better I think</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ntddv</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>18nsgka</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>I’m quite new to doing acrylics and it’s a nice hobby to have, here is my latest set in myself and I’d appreciate any advice!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mt7jkvq0po7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>18nsdjj</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>My choice for this christmas holidays🤭</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nsdjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>18ns6ic</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>New setttt by my AMAZING nail tech @nailsbycin . 🩷🩷</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wshs7qowmo7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>18ns3p3</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>🎀 A Pink Christmas 🎀</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ns3p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>18nryol</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>New weird Christmas set</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nryol</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>18nrvpj</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>In my country tradition has it that you have to eat pork in the New Year because the piggy will dig luck up from the ground🐷🩷</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ig8kpj5kko7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>18nrk3r</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Loving the colorcombo on todays client!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cji8bsz0io7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>18nrbpe</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>a different style</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8qxo546go7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>18nqw7b</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I'm absolutely in love with my Christmas nails! By Snappy Nails.</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nqw7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>18nque1</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Any tips on how to get a better polish application?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nque1/any_tips_on_how_to_get_a_better_polish_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>18nqeug</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nqeug</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>18nqd7p</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Christmas 🎄💅🏼</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74xwwidj8o7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>18nqcdd</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Christmas Nails!!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wxu4nrc8o7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>18npwpg</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Hand painted holiday nails from the last couple of weeks</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18npwpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>18npd2q</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I keep blinding myself with this pink!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4in4kwvj0o7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>18np3ly</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>CHRISTMAS GEL-X … WHAT DO YOU THINK??</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7ham6aicyn7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>18nopxb</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>bodied</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nopxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>18nogby</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Finally! A successful gradient!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfv3kgb3tn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>18nog5o</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>South Florida Nail Supply?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18nog5o/south_florida_nail_supply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>18noc40</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Christmas claws</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mklurfo4sn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>18nnxge</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Reflective X-Mas Mani</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nnxge</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>18nmqtl</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Slime nails</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wfv8ot8en7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>18nmgzk</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>which shape suits me more?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nmgzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>18nm1sx</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Candy Canes 🔴⚪️</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nm1sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>18nlsyk</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Control your excitement - it's more Christmas nails! And they're press-ons!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nlsyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>18o9rvi</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Whats your favorite ppu grabs this year?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o9rvi/whats_your_favorite_ppu_grabs_this_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>18o9p1e</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>I have never been so organized in my life!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o9p1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>18o9nsa</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Mooncat Magnetic Help?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o9nsa/mooncat_magnetic_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>18o8ixk</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Are my nails okay?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ogpl6unjs7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>18o8hlx</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>is this normal for new polish?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o8hlx/is_this_normal_for_new_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>18o8dxx</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Finally figured out magnets!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4837664is7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>18o59sg</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Mani Mad Science - Magnet Maximization</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2atra4wolr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>18o85jl</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Matched my nails to my NYE dress</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slr6qhpifs7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>18o706w</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Freehanding a French tip is hard, as is cleaning up red glitter polish.</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o706w</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>18o6bk3</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Christmas mani 🎄 inspired by a post I saw on Reddit</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5kx47g3wr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>18o65y8</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Festive Snowflakes</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o65y8</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>18o5vx3</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Apres Gel X Tips</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o5vx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>18o5jwi</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Guys please help lol</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o5jwi/guys_please_help_lol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>18o5aka</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>wintery mani with a snowy accent !💙🩶❄️☃️🌨️</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o5aka</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>18o59n8</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Still No F*cking Excuse</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o59n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>18o5265</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Absolutely hypnotized by Sea Siren</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o5265</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>18o41zg</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Roll Call- Lacquer Count</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o41zg/roll_call_lacquer_count/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>18o3rwo</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>My collection of the loved/hated Revlon Perfumerie polishes!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgrdvg8r7r7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>18o3mkk</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Painted a couple days ago.. loving the Christmas vibe🙂🎄</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsn3ayuf6r7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>18o2xt4</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Help identify this gorgeous holiday red ♥️</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o2xt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>18o2h8f</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>"Is that the Italian flag?" or, Why I had to add some detailing to achieve 'festive holiday nails'</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5o28euhvq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>18o1b6a</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time on my own 🥹 Not perfect, but nothing more practice won’t fix.</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o1b6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>18o14f2</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Can I use Sally Hansen miracle gel with no top coat?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o14f2/can_i_use_sally_hansen_miracle_gel_with_no_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>18o0lvp</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Should I send back my Bluesky at home gel kit?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o0lvp/should_i_send_back_my_bluesky_at_home_gel_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>18o0lfb</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Last Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o0lfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>18o0is0</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Stamping and Sienna</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18o0is0/stamping_and_sienna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>18nzy0u</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>u/christmascrazyyy posted a red, pink, and green mani, so I posted a red, pink, and green mani 😉 Thx for the inspo!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljlvlfb7bq7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>18nzqkc</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Scalper/price gouger on Mercari</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nzqkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>18nzjff</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>This shade is so pretty. It’s like what aliens eat on their toast.</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wb8xqe38q7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>18nzeu7</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Forgot to add the pic. Lol</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnyppwr37q7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>18nzd0d</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Are pink and teal Christmas colors?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz3zi4hp6q7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>18nywv2</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Holo pink/brown leopard nails</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nywv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>18nvf5w</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>After 4 months of not biting my nails, I’m finally confident enough to show off my nails!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nvf5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>18nyfov</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Mooncat Haunted Forest 💚</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7m1zii9zp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>18nydqe</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Grinch Nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nydqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>18nych5</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Winter Solstice Shimmer ✨</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nych5</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>18nxzj1</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>It’s my mom’s birthday! Help me give her a little peace of mind💝</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nxzj1/its_my_moms_birthday_help_me_give_her_a_little/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>18nxtlv</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Comp request: Mooncat - Heavenmetal vs BKL - I Will Devour All of You</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nxtlv/comp_request_mooncat_heavenmetal_vs_bkl_i_will/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>18nxsmn</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>I was going to do Christmas nails, but…</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nxsmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>18nww8d</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Working through my Black Friday haul</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd60oll9np7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>18nwu8y</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Recap? More like year long diary of every manicure/nail prep I did all year.</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dly2b9aump7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>18nvzgo</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Christmas Mani + this years faves</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nvzgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>18nvl9g</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>this texture makes me want to scream</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jk1b0ye2dp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>18nvgqm</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Painted these a couple days ago so they're a little worn now, but I've gotten so many compliments on this red!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9h9wts3cp7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>18nuzs7</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>A Little Midnight Gobble</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nuzs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>18nuz33</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Which nails should have art?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nuz33/which_nails_should_have_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>18nu4dc</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Finally getting festive!</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gguu0lv1p7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>18ntsmi</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Vibrant and festive!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ntsmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>18ntrwr</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Tis the season...or whatever</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y240vvk7zo7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>18ntjfi</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>can’t make nail art uniform so just went abstract instead</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gllmfj3fxo7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>18nsf88</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>ISO A true, mid century style frosted shell pink nail polish. I want it to be as close to your grandma's fave shade as possible and available in the UK</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gca2aj2qoo7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>18nrprk</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Multi-chrome magnetics might have become my favorite type of polish 🤤</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nrprk</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>18nr9vo</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Dupe-ish</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nr9vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>18nqp8f</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Tried this nail polish again with a stronger magnet and I’m so glad I did!!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nqp8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>18nqcj2</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Holiday Nubbins</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wrnvnxd8o7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>18nq37y</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Swatch request: Essie Willow in the Wind &amp; Cirque Matcha</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nq37y/swatch_request_essie_willow_in_the_wind_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>18nq2h3</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Christmas nails! 🎅🏻 🎄</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efd0r3ha6o7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>18npyqr</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>they are GLOWINGGGGG</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18npyqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>18npkem</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>INLP sweet pea</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18npkem</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>18noy6p</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>weird transparent patch on my ring finger - why and anything i can do to get rid of it/prevent it?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18noy6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>18nopl2</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Playing around with magnets</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nopl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>18no8af</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Oxytocin 🔥😍</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdyla4t8rn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>18no2df</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Wanted winter not Christmas ❄️</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qp0hnd7tpn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>18no1rx</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Trying to recreate dupes on my no-buy</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18no1rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>18nne6h</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Festive 🎄</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr4x15v2kn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>18nn8nu</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Joy is bringing me so much Joy</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ybxa33pin7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>18nbrip</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Christmas Nail design help!!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwt8423c4k7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>18ndmls</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>In April, I only owned 10 Essie Expressie Polishes.</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6tiazpslk7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>18nmngh</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>ILNP - Ruby</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nmngh</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>18nmn70</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>This is what my nails look like when I take the polish off. How do I fix that?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge8bkl4adn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>18nm4b9</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Mooncat I'm a MF Supernova</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nm4b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>18nlxm1</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Didn’t mess up my drying nails for once</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0hp2osc6n7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>18njfa8</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Help finding regular polish dupe for these shades.</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18njfa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>18nii7v</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Zoya Katherine vs Essie Bordeaux</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18nii7v/zoya_katherine_vs_essie_bordeaux/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>18o8a9e</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Icy Christmas set</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwwd83fygs7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>18o83bb</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Baldur's Gate 3 Themed Nails -Astarion-</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o83bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>18o7jq9</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Found better lighting</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o7jq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>18o5r94</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Glow in the dark Ombre Nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o5r94</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>18o5oin</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>🎆</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcu7lfyrpr7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>18o224w</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I love how the middle finger turned out!!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18o224w</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>18nzlew</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Some recent nail sets I’ve done</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nzlew</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>18nw9ib</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Blue chrome Christmas</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nw9ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>18nuu72</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>A little early to New Year’s</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hypiudaa7p7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>18nr2tl</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>I'm absolutely in love with my Christmas nails! By Snappy Nails.</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nr2tl</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>18npzln</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Hand painted holiday nails from the last couple of weeks</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18npzln</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>18np5v6</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>A little sparkle action ✨</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xphjypvyn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>18nmm06</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>How to do matte on top of gloss?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gpzvm7ycn7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>18nme8u</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>After a massive fail, I achieved my Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nme8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>18nlbpm</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Christmas nails pt2 ❄️✨</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nlbpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>18nkpq0</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nkpq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>18nimuh</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>KUROMI-CHAN!! 💜🔥💀 by yours truly.</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsg167y64m7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec 23 08:07:01 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_24.xlsx
+++ b/data/2023_12_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C949"/>
+  <dimension ref="A1:C1127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16566,6 +16566,3032 @@
         </is>
       </c>
     </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>18p0rx6</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>First time painting fake nails and doing ombre, I think they turned out pretty good!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18p0rx6/first_time_painting_fake_nails_and_doing_ombre_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>18p0nk1</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>My christmas nails this year</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p0nk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>18p0jl1</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>I hate my nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p0jl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>18p0goz</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Peel off latex safe in uv lamps?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5qq4j7cyz7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>18p08wc</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Not bad for $1.50 press ons 🤩</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p08wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>18ozvmx</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Clear top coat peeling off press on nails. What do?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg1nzr94rz7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>18ozrld</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Got a new set to compliment my skin tone</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd1onoespz7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>18ozbdn</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>What is the best way to strengthen your nails?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ozbdn/what_is_the_best_way_to_strengthen_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>18oyil8</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>nail biting feels like a never ending cycle, please help</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18oyil8/nail_biting_feels_like_a_never_ending_cycle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>18oy3ko</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Holo taco frost light for the winter!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5al9qdp7z7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>18oy21n</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>My First Attempt at Nail Art 😅</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oy21n</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>18oxu6g</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>She’s so talented! Cinderella nails by mooyahyahh on YouTube!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k45kdc5n4z7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>18oxqpd</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Snowflake nails for Christmas!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oxqpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>18oxq7v</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Slay nails.... sleigh nails..</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oxq7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>18oxaun</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Holiday-ish Naisl (i hate the color)</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oxaun</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>18owhwy</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>First French tips I’ve ever done!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18owhwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>18ow91l</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Is this dark red or red wine?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ow91l</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>18ow5y1</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>First nail design I have ever gotten! Can pink be a Christmas color?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yok7iwhpny7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>18ow3x3</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Interested in getting a set like this. Does anyone have any ideas what something like this may cost and how long it would take. Busy girl on a budget.</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4b15la5ny7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>18ow25m</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Where do I get these smaller pointy swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aurswonomy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>18ow0ph</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Christmas!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ow0ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>18ovvgs</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Nubbins</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgmjoo3uky7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>18ovr4s</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>cashmere cat eye for the holidays ❄️</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jbhx8jpkjy7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>18ovq2h</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>natural nails lounging in my new room. 🥀🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8b7ux3hbjy7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>18ovmy8</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Wreath nails</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kllk6zeiiy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>18ovma3</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Never gotten rhinestones on my nails before, I’m NOT use to this texture 🤣 But I like them! I couldn’t decide what to do for NYE.</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9z7whhbiy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>18ovklb</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>First polygel set!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ovklb</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>18ovh9g</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Holiday nails 💅 🎄</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gatqcsxgy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>18ovh7p</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>New ombre solar nails</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ovh7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>18ovdkw</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>All the nails I’ve done this year.</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ovdkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>18ov6lr</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>First acrylic full set on myself!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ov6lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>18ov3l9</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Holiday Nails 🎁</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ov3l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>18ov20n</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Just Realised my holiday nails are also in tribute to my favorite beverage</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etnqc43ucy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>18ov13k</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New years nails! </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/os721sdkcy7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>18ouz36</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Get my nails done once a year.. I love ‘em!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ouz36</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>18oul9r</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oul9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>18ouhme</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Did my own gel manicure for Christmas (not a pro; just a hobby) … What do you think?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04lqt6ei7y7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>18ou378</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Miffy nails</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jedqkzhr3y7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>18ou2sw</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>No such thing as too much glitter ✨</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xohgm4mn3y7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>18otsmz</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3swwmry21y7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>18otrib</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>First time ever getting my nails done! Summer Christmas ❤️</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18otrib</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>18otnsb</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Pottery nails</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18otnsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>18otmlq</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Any other things I need to get that aren't included in this kit?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btf7hnxgzx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>18otheh</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>NYE</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18otheh</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>18otbnc</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Asked for a French tip…</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7efze7qwx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>18ot8w7</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Xmas nails DIY</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2dkxfn0wx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>18ot6cx</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>I’m still in love with my wintery set (gel x by me)</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ot6cx</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>18osog6</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Help making tweaks at home?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18osog6</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>18osjkw</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Is this color festive enough? 😅</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wq2x0uvpx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>18osht3</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Buuuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tzvhhlgpx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>18osd26</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>I did my first Gel- X set and I’m super proud of myself 🥹</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18osd26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>18os8n5</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>❤️🎁🎄</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18os8n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>18os7fu</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>what my salon did vs my attempt at fixing it. does it atleast look a little better? I didn’t have time to get them redone today so i just tried to make them look a little better myself.</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18os7fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>18ortnz</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Gel nails w chrome powder.</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ortnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>18orrlx</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Still waiting for my Christmas color to come but I desperately wanted a fill &amp; now I'm obsessed with my natural nails 🥲</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18orrlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>18ornus</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Did my holiday nails and I’m not sure i like them what do you think?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o7geg1bix7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>18ormsw</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>What do you think about my new nails!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ormsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>18orcvm</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Chrome babies</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18orcvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>18oqs9g</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Refreshed Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oqs9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>18oqg0t</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>What are people’a opinions on natural unpainted long nails?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms2iur028x7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>18oqd97</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Sparkly for the holidays</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smklsyrd7x7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>18oqamr</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Are these giving winter/christmas?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oqamr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>18oq96q</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Who said short nails can't be cute!?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oq96q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>18oq7f2</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Nothing like a fresh set</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnirfuc16x7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>18oq12b</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>I asked my son (5) what I should do; he said “blue on the left, right on the pink”. Heading home &amp; cant wait to show him! 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oq12b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>18oq0yb</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oq0yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>18oq07t</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Gold chrome for Christmas!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oq07t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>18opofe</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Christmas sweater</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18opofe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>18oplff</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Finally got around to getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq29x5kz0x7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>18opgse</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>My simple Christmas nails❤️</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18opgse</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>18oovrs</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>💚❤️ ILNP Holiday Bundle 🎄✨ Two coats each of Say Love, Fir Coat, and Empire</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oovrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>18oouh8</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oouh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>18oos22</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>holo taco "wicked potion"</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ckxys64uw7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>18oosnx</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>If you do a two color manicure, do you change color every finger or do you do one color for middle and ring finger and the rest in the other color</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gggn5wpbuw7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>18onv4v</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jnppthgmw7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>18onnmw</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Love the color of my most recent set ❤️</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnsh4pookw7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>18oni5x</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>I scuffed my nails already sadly, but they’re so gorgeous and were even more gorgeous when first done.</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oni5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>18on67g</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Proud of how far I’ve come doing my own nails in the last year!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18on67g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>18omw0k</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>No Christmas nails. Decided on pink nails with sparkle to take me through to the end of Jan.</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8dwgw9aew7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>18ompof</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Have you ever broken a nail...</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ompof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>18omgmo</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Holiday set</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vh00u4maw7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>18om70c</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>nail growth from today &amp; last week! 🤭🖤✨</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18om70c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>18om5f3</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>My first attempt at acrylic!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18om5f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>18olwfe</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Tobacco smell cured in nails?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18olwfe/tobacco_smell_cured_in_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>18olwaj</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>New set for the holidays</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18olwaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>18ollgj</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Had to go to a Salon for my engagement nails.</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl6sp7dq3w7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>18oljzl</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Christmas Special Edition 😍💅✨ love them</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oljzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>18ol4p9</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Simple french tip winter holiday nails</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/e7cT2C2.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>18ol0at</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ice queen gel x aqua nails </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/azs8auh3zv7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>18okrvl</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Why do my nails peel only on the corners?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r0vlpkcxv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>18okyqz</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Can I ask for dips with no UV-cured top coat?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18okyqz/can_i_ask_for_dips_with_no_uvcured_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>18ohedx</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>jelly acrylics nail art ideas ? (Inspo @nailjob)</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ohedx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>18okarq</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>My reflective French Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quyez3gmtv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>18okac8</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>3 months of progress</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zr36039jtv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>18obsu4</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Brittle nails but i wanna keep getting them done</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18obsu4/brittle_nails_but_i_wanna_keep_getting_them_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>18nzkk7</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Opinions? Are these considered XMAS nails? Inspo by @karina_capricorn777 on Instagram.</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18nzkk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>18ojxl6</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>do they look horrible as i think be real</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ojxl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>18oj51g</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Each nail is a different design ❤️🌲 my right hand isn’t as cute so just posting my left lol</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oj51g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>18oj0h6</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>first set I’ve done in a while. going to keep practicing since these prices are getting out of hand</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oj0h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>18oi0e2</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Some chilly ice nails just in time for the holidays! Featuring cracked ice technique</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/09sattp1bv7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>18ozlev</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>I was going for gaudy</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbhjc0btnz7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>18oyx50</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>What did everyone get for BKL's Buzzmas 2023?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9702wqagz7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>18oyuc0</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Fix polish or start over?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oyuc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>18oyt2s</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>so ready for christmas!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvdgjwp2fz7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>18oy3c8</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>the christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oy3c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>18oxhkb</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>My Christmas nails (inspo from tessa.lyn.nails on insta)</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaotqhb81z7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>18ox2ne</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Vacation nails!!</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ox2ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>18ox0ql</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Dupe for Essie Sweater Weather?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrabmcmgwy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>18ow188</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Christmas time is here...</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ow188</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>18outcq</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Plum and gold glitters</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t56ezahkay7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>18ou40g</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>My nails for Christmas this year ✨</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ou40g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>18ot6u7</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Why does matte top coat only work on some of my nails?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ot6u7/why_does_matte_top_coat_only_work_on_some_of_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>18osl2g</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Is this color festive enough? 😝</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qe9mpgj9qx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>18osbj6</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Most Unique Mooncat Shade?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18osbj6/most_unique_mooncat_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>18os29f</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>New Years Nails :)</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcyejyenlx7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>18orxuw</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Merry Chrysler</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18orxuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>18orp7i</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Whatcha - Aurora Borealis</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ur9z72dkix7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>18ord6w</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>The sun came out ☀️</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ord6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>18orcpf</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>KB Shimmer Magnetics Velvetized</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/63vc2ckifx7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>18oqp9w</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>it's my Birthday tomorrow so I decided I wanted to go all out with the mani and freehand up a storm!! :)</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oqp9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>18oq6f1</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>My Christmas mani! Funny enough, my teenage bedroom was the same color combo.</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oq6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>18opsgb</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Simple holiday nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18opsgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>18opn2k</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>ILNP Magnetics Velvetized</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9wyps0d91x7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>18opcac</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Another Christmas mani 🎄</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w5s01euyw7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>18op7wc</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Christmas nails and first time doing French tips❤️</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18op7wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>18op5kl</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Day 8 and I finally take a picture</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18op5kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>18ootz7</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>💚❤️ ILNP Holiday Bundle 🎄✨ Two coats each of Say Love, Fir Coat, and Empire</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ootz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>18oo2a4</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Emily De Molly Magnetics Velvetized</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/khokstq3ow7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>18onqqd</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>My take on the Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnylpicflw7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>18oneno</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Cirque Magnetics Velvetized</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7nxggoggiw7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>18omhyq</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Yes, it's a WFL PPU polish. You know which one.</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18omhyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>18ombqb</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Ahhhh, ok fine, you all inspired me, I did a red manicure for the holidays 🤣</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzjco2bi9w7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>18om9h7</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Todays nails :)</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18om9h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>18om71y</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>To anyone who's got this product, what's your experience with it?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gk7flw5k8w7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>18olsf8</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>I’ve had the almond shape for years and a friend convinced me to try coffin. Is it more flattering for my hands?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18olsf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>18olfjn</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Mooncat Whiskey Sunrise ✨️</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18olfjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>18ola5d</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Simple french tip winter holiday nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/e7cT2C2.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>18okzhs</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>My simple holly jolly manicure 🎄</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18okzhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>18okv73</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Need help finding nail polish similar to Psilocybin (Clionadh Cosmetics)</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18okv73/need_help_finding_nail_polish_similar_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>18oktn1</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Why do my nails peel only on the corners?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rixygufqxv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>18okoz4</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Got a New Year’s idea in my head &amp; scrapped my Xmas nails early!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18okoz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>18ok3j9</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Why does this keep happening</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqrz2c50sv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>18ojvxo</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Soft and cozy for the chaos of the holidays</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ojvxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>18ojv2l</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Polish org/tracking apps you’d recommend?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2s252t2qv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>18ojtvr</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Did Velvet swatches of all my PPU magnetics</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kindabfspv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>18ojkku</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>This year I didn’t want such traditional christmas nails 🩵</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2avselrnv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>18ojjxj</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Perfect color for a foggy morning! Morning tide jelly 🌊</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ojjxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>18oj9kq</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>My version of Xmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oj9kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>18oj6nh</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Holiday polish disaster?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18oj6nh/holiday_polish_disaster/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>18oj35q</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>random skittle before christmas🍒🍷🫧</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oj35q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>18ohw1v</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>To any thinking pink and teal aren't "holiday" enough...</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ohw1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>18oh6c8</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>PSA: fishing for nail compliments in the group chat may lead to polish parties</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oh6c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>18oh2se</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Yum polish, so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/CIrikt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>18oghc3</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>DIY white christmas ☃️</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tof7uqh8zu7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>18og5oh</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>My Christmas nails for this year!!! 🥹🎄❤️</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18og5oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>18og4my</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>ever spend the better part of your day getting the perfect shape, just to paint them and not be totally satisfied? 😩</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18og4my</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>18ofe0r</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Christmas Nails (part one)</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xq7jcjwpu7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>18oet80</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Velvetized Jet Setter</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qfrspg6qku7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>18oe2m1</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>My take on Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oe2m1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>18ody70</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Which magnetic polishes are good for the velvet effect?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ody70/which_magnetic_polishes_are_good_for_the_velvet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>18oao1x</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Finally got my press-ons to stay! Now, how do I get them off?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iitgqfbat7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>18p0rgc</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfy07ic6208c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>18p01mw</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Securing charms</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/18p01mw/securing_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>18oy0y6</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>A set I just finished!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s508t2ru6z7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>18oxfkm</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I need a little help!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/18oxfkm/i_need_a_little_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>18owb98</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Week old full set i did (beginner)</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1ho4kw5py7c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>18ovttz</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Christmas nails ❄️🎄</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/13ras8u6ky7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>18oveiy</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Just a little snowy friend ☃️</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gtfrfyq5gy7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>18ovanr</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Building up my nail binder</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g83hd8p5fy7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>18ov0dk</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>New years nails!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y8i6ohkdcy7c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>18osbvy</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Pink dreams✨💕</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tidqfh1ox7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>18opf8a</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>My simple Christmas nails❤️</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18opf8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>18ooiq7</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Repost 😭 Christmas Press Ons I Made</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ooiq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>18oncqj</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Christmas nails by @aisancenailstudio</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oncqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>18omk19</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Some press ons I’ve been working on this week</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18omk19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>18oja1u</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My nails for the holidays😊</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2i34xlilv7c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>18ofyb9</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>my design for these dates. Doesn't it look adorable?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ofyb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>18odj9v</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkxvsia38u7c1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 24 08:07:34 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_24.xlsx
+++ b/data/2023_12_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1127"/>
+  <dimension ref="A1:C1307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19592,6 +19592,3066 @@
         </is>
       </c>
     </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>18ppy9w</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Feeling Christmas ready</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3dyhgfyjz68c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>18ppr5g</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Builder gel question</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovhl7ar5x68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>18pplvb</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>First timer!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywhnvaeev68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>18ppjn5</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Tried budget polygel…..never again</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvgt7ppou68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>18posrg</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Santa hat nails 🎅🏻</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otza2uixl68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>18popj8</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Simple red dots</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptapzfhzk68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>18poj39</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>New years nails!</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18poj39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>18poepj</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Miss my Halloween set</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zkn5djrh68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>18pnumg</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Most recent set for the holidays</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pnumg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>18pmoid</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>weekly nail growth update 💅✨</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pmoid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>18plr80</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Is it normal for dip nails to change colors? Or was the lighting in the nail salon just totally different?</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18plr80/is_it_normal_for_dip_nails_to_change_colors_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>18pkp9g</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>extremely damaged nails.. help</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pkp9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>18pjbq2</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Nail salon downtown / soho nyc</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pjbq2/nail_salon_downtown_soho_nyc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>18pgp6b</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Second and best attempt at pottery nails (inspired by Oaxacan pottery)</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pgp6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>18pff8h</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Dramatic before and after</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pff8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>18pnfs3</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>My sister did my nails!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pnfs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>18pn4ze</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>How did I do with these Glue Ons?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pn4ze</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>18pmgx9</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Polish completely peeled off acrylic day after getting them done</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pmgx9/polish_completely_peeled_off_acrylic_day_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>18pm59a</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Hand painted</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pm59a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>18pm4qh</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Change but I like them</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9err5o5ot58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>18pl6ky</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Had to show off my Christmas nails. Happy holidays everyone 🎄</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbx616m3k58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>18pkwuk</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Merry Christmas! 🎄🎅🏼</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ue4e68ueh58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>18pkd58</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>I can’t paint my nails!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pkd58/i_cant_paint_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>18pk0p6</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>I said I wanted stars and lime green and this was the outcome! Love my nail artist 💚</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixwz7rjo858c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>18pk0p0</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Feeling festive! 🎄✨</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agfbzxeo858c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>18pjfaw</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Love this nail set!!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wp0fcd1358c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>18pj14x</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Tiny reindeer nail art with snow speckles, handpainted on me by me</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnnzdncgz48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>18pj0hs</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Christmas nails that took longer than they probably should have!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v69izmaz48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>18pit61</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>[M30] First time getting my nails done in public</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pit61/m30_first_time_getting_my_nails_done_in_public/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>18pilc4</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Last set of the year!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xbwavikv48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>18pi6t9</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>simple &amp; clean</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knuxd0ixr48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>18phxrt</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>best press-ons?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18phxrt/best_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>18phbxp</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Finally did some Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brzvfigek48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>18ph8mc</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>The longest my natural nails have ever been!! (don't mind me rocking like three different nail shapes, I don't have the heart to file them all down when one breaks)</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ph8mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>18ph3bo</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Booked for gel nails but got acrylics instead</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ph3bo/booked_for_gel_nails_but_got_acrylics_instead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>18pgr9g</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>New set 🪩</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6q29yo6f48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>18pgo48</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Getting into the Christmas spirit</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh844i8ce48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>18pghdg</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>My nails for this holiday season</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rig271loc48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>18pgh9p</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>DIY long stiletto nails?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pgh9p/diy_long_stiletto_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>18pgg84</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noeu438hc48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>18pgb6l</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>I’m not usually one for regular polish but this is so pretty💙</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pgb6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>18pgazd</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I debulked and changed the base color to a sparkly purple ✨</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knui69s7b48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>18pg07v</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>I think my nail beds are unusually short and wide. Are they?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0yrfd5k848c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>18pfw8z</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Happy holidays! (Very amateur hand painted design)</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pfw8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>18pfqz1</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>my nails are ready for Christmas!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a69nh2ea648c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>18pfml7</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Feeling Blue</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zoojtm68548c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>18pf8gd</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>It happened - nails are grown out but OMGGGG</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h8jt3kv148c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>18pf8c9</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uig3jhfu148c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>18pf2xf</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Christmas set DIY mani.</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z00cv9kj048c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>18pet16</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>This was my first ever time putting rhinestones on a client and I’m not entirely mad with how they came out! Though, I will work on the placement of the rhinestones for the next set I do</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3um7c6g7y38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>18pec49</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Gel polish chipping?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pec49/gel_polish_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>18pe9gd</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>How does this happen?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yrb286kt38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>18pe8o7</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gt4torct38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>18pe8n4</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Husband surprised me with a Holo Taco collection box for Christmas!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g130mjct38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>18pdsrg</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Help! How to fix builder gel chip?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omud4nqkp38c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>18pdl12</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Vacation time!! I felt like something fun for my upcoming trip to Jamaica.</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pdl12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>18pcl76</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>nails wrapped 2023</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pcl76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>18pdg60</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Simple set for christmas :3</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pdg60</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>18pdfuu</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f45wkejm38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>18pdenj</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>My nail tech did so good ❤️</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcf3cb79m38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>18pd6f7</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>something simple and classic for the holidays (my thumb nail broke so rip)</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgsihzz9k38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>18pcwtn</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Shein semi permanent polish</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pcwtn/shein_semi_permanent_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>18pcohq</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Christmas</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pcohq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>18pci66</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Two days before Christmas but missing summer.</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pci66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>18pc7he</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Recently got into doing my own nails and loving this simple holiday set!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cshc78mzb38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>18pbka1</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Press-Ons (Light Pink)</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pbka1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>18pbjmq</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Blue Chrome 🩵</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1j0l7jf638c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>18pbam7</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Sparkly nails ✨</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hezd9uta438c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>18pb9n9</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Let it snow ❄️</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4pec3a2438c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>18pb0ch</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Nails dipped in gold?!</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j0159uv138c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>18pazb6</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pazb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>18pal4k</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Help - weak, brittle nails that I bite. Would extensions help?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18pal4k/help_weak_brittle_nails_that_i_bite_would/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>18pa675</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Christmas nails :D</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up8fppjou28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>18pa42s</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Super curved nails</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgman3a7u28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>18p9zas</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>My Mom has been a natural nail queen since 1978</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z23y8533t28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>18p9w5b</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Press-on appreciation post !!!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p9w5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>18p9t8b</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>I’m very upset</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riywgownr28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>18p9t39</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Glitter and Pearl</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p9t39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>18p9psr</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>My Christmas Nails 🎄🦌</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kb00uk3wq28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>18p3uqr</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Need Nail Help!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18p3uqr/need_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>18p3o1s</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Nail health help</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18p3o1s/nail_health_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>18oy3yy</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>christmas tree nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18oy3yy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>18ouzgs</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>First time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ouzgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>18oo0d2</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Why is my colored gel "peeling" when filing down?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18oo0d2/why_is_my_colored_gel_peeling_when_filing_down/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>18p8l3m</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Christmas nails courtesy of Glamnetic ✨</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31xa32t5h28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>18p8f9e</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Last holiday set of 2023!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p8f9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>18p7n1v</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>First time getting french :)</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2am95sg4928c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>18p77v2</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Plain and simple 🤍</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p77v2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>18p70m2</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Yesterday's manicure 🧑‍🎄✨Holiday nudes✨🎄Gel polish on my natural nails.</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avtogr1y228c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>18p6v0c</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Have I been had?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p6v0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>18p6onl</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Last Christmas Set 🎄</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p6onl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>18p5oth</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Red Nails for Christmas❤️</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5dp861qq18c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>18p5c49</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Help with doing gel x at home</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18p5c49/help_with_doing_gel_x_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>18p56wl</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Pink Christmas nails ft cursed grip</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl5iezzll18c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>18p4h14</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>My simple festive nails</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p4h14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>18p4b8o</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>My natural nails, I do them once a week myself!</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jas6ybfkb18c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>18p3oog</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Simple Christmas 🎅🏻</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vc9cedb418c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>18p3gvs</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Rate them!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p3gvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>18p1bc7</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Not sure if I'm happy with the result..</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p1bc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>18pqqnz</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Spray Paint</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18pqqnz/spray_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>18pojg8</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Pahlish Fill Line Issues (Warning: Second photo is a mystery polish)</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pojg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>18pnqym</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Christmas manicure</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td1s33vqa68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>18pnkvk</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>UV polish in action!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vcyev09w868c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>18pnk5w</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>ILNP Roulette</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srtxu94q868c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>18pjf5j</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>First time nails, holiday style</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvatu7qz258c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>18peuwq</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Sticky layer of my colour gel messes up my top gel</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18peuwq/sticky_layer_of_my_colour_gel_messes_up_my_top_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>18pnbfh</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>BKL Buzzmas days 1-3</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pnbfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>18pn7xt</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Whar ~300 Polishes on a Wall Looks Like</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nifz2pc9568c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>18pmd1v</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>First time trying cute stickers on top of polish :) santa gotta a little messed up, but little gingy on my pink is ok, so I'm ok 💖</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rka8v8b5w58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>18pm9ie</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>ILNP “Joy”</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnltyvo2v58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>18pm54i</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Merry Christmas everybody!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pm54i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>18plxhb</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Tips/ Advice</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2yggzumr58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>18plqh6</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Today I panned a nail polish bottle</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18plqh6/today_i_panned_a_nail_polish_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>18plkt1</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>This year's Christmas mani is green with reflective glitter</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/daiy9g9un58c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>18plirt</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Reccs to fix yellow nails?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6oe7qeajn58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>18pki05</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>“Corinna” (Zoya)</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8rgicded58c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>18pjyyz</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp2pjim6858c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>18pj800</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Snow Much Fun</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty4rx376158c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>18pj71j</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Christmas Mani...and my first time trying nail art</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pj71j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>18pj5w6</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust ✨️</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pj5w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>18pj1rz</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Where can I find a Magnetic clear thats not gel.</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18pj1rz/where_can_i_find_a_magnetic_clear_thats_not_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>18piygl</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>My Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ynkrt5ty48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>18pimz2</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Good Fortune by ILNP with Foxfire topping by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5wajrasxv48c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>18pihhd</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>My Wildflower Laquer Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1x797smu48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>18pibna</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Christmas nails ft Sally Hansen Red It Twice and Illamasuqua Rampage</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1ocr8u5t48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>18phqia</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Truth is Painful</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnf89swwn48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>18phjrf</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>First set I've ever done myself!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f3wtj49m48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>18ph79w</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Christmas Plaid</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ph79w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>18ph3wk</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Sold out polish</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ph3wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>18pgnem</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Christmas nails 2023</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ra5aeh7e48c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>18pghkg</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Update: Thanks to all the advice I got from you Laqueristas, I succeeded at not flooding my cuticles.</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pghkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>18pg3hw</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pg3hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>18pg17c</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>All wrapped up</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwqk7mft848c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>18petvb</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Christmas Manicure 🍒🎀</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5z2i7yey38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>18pep6u</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Sally hansen it takes two</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8enjyksax38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>18pe2n8</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Grownups like numbers... but we like cats too 😹</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pe2n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>18pdv4y</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Christmas Nail Art</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pdv4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>18pdkup</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pdkup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>18pdjhz</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Lily and Fox Nail Wraps?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18pdjhz/lily_and_fox_nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>18pcw33</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>What is the best lighting to show off nail polish and why is it inside a car?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra51o6vuh38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>18pco6r</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>oldie but goodie</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg60h61xf38c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>18pcmmh</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Wild Berry West + Holo Taco - Lunar Unicorn Skin</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pcmmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>18pc7i5</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I showed her this dress and told her she could do what she wanted as long as she followed the color scheme. I think she did great</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pc7i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>18pbhix</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Pre Christmas Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pbhix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>18pb4s8</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>LPT: If you do a single accent nail, always paint it first!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18pb4s8/lpt_if_you_do_a_single_accent_nail_always_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>18paw5r</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Question how to clean glass nail file while using it?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18paw5r/question_how_to_clean_glass_nail_file_while_using/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>18pavkf</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>This green arrived just in time for a simple Christmas mani</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pavkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>18patch</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Can anyone identify so I can match my toes to my nails?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sam4tdw7038c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>18pa8u6</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Not exactly holiday nails but they make me happy ✨</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pa8u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>18pa7ly</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>a different color scheme for christmas ✨💜</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pa7ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>18p9qjm</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>My Christmas Nails 🤶🎄☃️🦌</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ej5s4bzq28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>18p9m66</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>My Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7s35f961q28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>18p9gjl</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Green for Christmas</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p9gjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>18p9ckv</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Helllloooo to my first shrinkage.</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dapqma1nn28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>18p8wio</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Nail Oil Tools &amp; Recipe</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yklufqbj28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>18p8l4g</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>My Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p8l4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>18p86pg</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>I don't have proper greens, reds, or golds, so I did blues</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p86pg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>18p7n9x</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Is it weird to bring a glass file to a nail salon appointment?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18p7n9x/is_it_weird_to_bring_a_glass_file_to_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>18p7dqq</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Inspired by all the beautiful holiday manicures, I decided to give it a try!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18p7dqq/inspired_by_all_the_beautiful_holiday_manicures_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>18p79rr</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Obligatory Christmas Manicure</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psj7zzzs528c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>18p74iw</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Christmas vibes 🎄</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8xf9qcd428c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>18p714n</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Xmas Mani 2023</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p714n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>18p70v5</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Stardust by Olive Ave Polish</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noo1y3th328c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>18p5gbo</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>🎶A beautiful sight...🎶</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0680icn9o18c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>18p2tn9</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>In protest of red &amp; green, and all alleged “winter colours”</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18p2tn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>18p26gc</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>dry streaks from inm top coat</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d37oqyqok08c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>18po95p</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>My sister painted my cats on my nails and I can’t believe it</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18po95p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>18pnx7c</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My first time trying nail art. I’m obsessed. Thoughts? Constructive criticism? Tips?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypj5hnbnc68c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>18pltjn</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Nail Art</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pltjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>18pj45s</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Tiny reindeers galloping on baby pink, snow-speckled background, handpainted by me on me</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfsqbth7058c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>18pe1zc</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>My and my husband's Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pe1zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>18pdtac</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Just did my Christmas nails!🎁</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pdtac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>18pdnq0</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>All of the holiday nails are so beautiful but I wanted something a little more fun for my girls trip to Jamaica. Huge thanks to my NT Irina @ Lash n Nail Room!! She's the absolute best!</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pdnq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>18pblgf</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>I gave myself New Years nails (gel)</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pblgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>18pbdxh</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Glow in the dark nails and dollar nail art 😏. Made by me 🌟</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d4jl472538c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>18pam8e</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Christmas</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pam8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>18pag8m</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Pearls are def my new obsession</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovoe4p43x28c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>18pafr9</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>In love 💕</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18pafr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>18p7lua</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w4gqfm1u828c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>18p39xd</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Very proud of this christmas set! Would love some constructive criticism</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jubcqzl9z08c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>